<commit_message>
State Management libs for Ng
</commit_message>
<xml_diff>
--- a/cheatsheets/ng/state.management.solutions.assessment.xlsx
+++ b/cheatsheets/ng/state.management.solutions.assessment.xlsx
@@ -44,6 +44,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lesbarkeit
+Pflegbarkeit
+Debuggbarkeit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schulnote,
+kleiner = besser</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -54,7 +85,8 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Importance of the above criteria</t>
+          <t>Importance of the above criteria
+higher = more important</t>
         </r>
       </text>
     </comment>
@@ -93,16 +125,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Boilerplate</t>
   </si>
   <si>
     <t>MobX</t>
-  </si>
-  <si>
-    <t>DIY
-Service / Facade</t>
   </si>
   <si>
     <t>NgRx</t>
@@ -130,10 +158,6 @@
     <t>Community</t>
   </si>
   <si>
-    <t>additional benefit: immutability built in
-de-facto standard for Ng Apps</t>
-  </si>
-  <si>
     <t>Weight:</t>
   </si>
   <si>
@@ -144,12 +168,6 @@
   </si>
   <si>
     <t>Result</t>
-  </si>
-  <si>
-    <t>not only for Ng Apps, not redux-like, is generally applicable!</t>
-  </si>
-  <si>
-    <t>easier-to-use alternative to NgRx</t>
   </si>
   <si>
     <t>why seldom (?) recommended:
@@ -157,13 +175,105 @@
   </si>
   <si>
     <t>Learning curve</t>
+  </si>
+  <si>
+    <t>DIY RxJS
+Service / Facade</t>
+  </si>
+  <si>
+    <t>Maintainability</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">additional benefit: immutability built in
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+      </rPr>
+      <t>de-facto standard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for Ng Apps</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+      </rPr>
+      <t>not only for Ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Apps, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+      </rPr>
+      <t>not redux</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t>-like, is generally applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+      </rPr>
+      <t>easier-to-use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Agfa Rotis Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; light-weight alternative to NgRx, still Redux-style</t>
+    </r>
+  </si>
+  <si>
+    <t>importance of the above criteria, higher = more important</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +312,24 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Agfa Rotis Sans Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Agfa Rotis Sans Serif"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Agfa Rotis Sans Serif"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -258,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -296,6 +424,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -588,64 +730,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.375" customWidth="1"/>
     <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="3.875" customWidth="1"/>
-    <col min="8" max="8" width="4.125" customWidth="1"/>
-    <col min="9" max="9" width="73.75" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="7" max="7" width="3.875" customWidth="1"/>
+    <col min="8" max="8" width="11" style="18"/>
+    <col min="9" max="9" width="4.125" customWidth="1"/>
+    <col min="10" max="10" width="73.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="28.5" customHeight="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.5" customHeight="1">
       <c r="B1" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
         <v>3</v>
-      </c>
-      <c r="C2" s="8">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8">
-        <v>2</v>
       </c>
       <c r="E2" s="8">
         <v>3</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="8">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="28.5" customHeight="1">
+      <c r="I2" s="9"/>
+      <c r="J2" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28.5" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
@@ -659,18 +812,21 @@
       <c r="E3" s="6">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="1">
-        <f>((B$2*B3)+(C$2*C3)+(D$2*D3)+(E$2*E3))/(B$2+C$2+D$2+E$2)</f>
-        <v>1.8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="15">
+        <f>((B$2*B3)+(C$2*C3)+(D$2*D3)+(E$2*E3)+(F$2*F3))/(B$2+C$2+D$2+E$2+F$2)</f>
+        <v>2.4666666666666668</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6">
         <v>3</v>
@@ -684,19 +840,22 @@
       <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="1">
-        <f>((B$2*B4)+(C$2*C4)+(D$2*D4)+(E$2*E4))/(B$2+C$2+D$2+E$2)</f>
-        <v>3.2</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.5">
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="15">
+        <f t="shared" ref="H4:H9" si="0">((B$2*B4)+(C$2*C4)+(D$2*D4)+(E$2*E4)+(F$2*F4))/(B$2+C$2+D$2+E$2+F$2)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.25">
       <c r="A5" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6">
         <v>4</v>
@@ -710,48 +869,54 @@
       <c r="E5" s="6">
         <v>5</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="1">
-        <f t="shared" ref="G5:G9" si="0">((B$2*B5)+(C$2*C5)+(D$2*D5)+(E$2*E5))/(B$2+C$2+D$2+E$2)</f>
-        <v>3.5</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15">
+      <c r="F5" s="6">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="6">
         <v>3</v>
       </c>
       <c r="D6" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="1">
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="15">
         <f t="shared" si="0"/>
-        <v>2.1</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -762,175 +927,196 @@
       <c r="E7" s="6">
         <v>2</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="1">
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="15">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15">
+        <v>1.9333333333333333</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="6">
+        <v>4</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="15">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="6">
-        <v>2</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="1">
+      <c r="G9" s="6"/>
+      <c r="H9" s="15">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>4</v>
-      </c>
-      <c r="E9" s="6">
-        <v>2</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>2.8666666666666667</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="H10" s="16"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="H11" s="16"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="H12" s="16"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="H13" s="16"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="H14" s="16"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="H15" s="16"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="H16" s="16"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="H17" s="16"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="H18" s="16"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="H19" s="16"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:9">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="H20" s="16"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F9">
+  <conditionalFormatting sqref="B3:G9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -942,7 +1128,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2">
+  <conditionalFormatting sqref="G1:G2">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -954,7 +1140,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E9">
+  <conditionalFormatting sqref="B3:F9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -966,7 +1152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:H9">
+  <conditionalFormatting sqref="H3:I9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -979,7 +1165,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I9" r:id="rId1"/>
+    <hyperlink ref="J9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>